<commit_message>
Estudo em python dia 16/09
Estudo em python dia 16/09 Pandas, Streamlit, plotly
- Tabela
- Coluna
- Query
- Documentação
</commit_message>
<xml_diff>
--- a/NY/ano_novo.xlsx
+++ b/NY/ano_novo.xlsx
@@ -1,12 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC YC\Desktop\Py\NY\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D38C5D2-D0B1-4396-A971-5075E78AA487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -67,9 +88,6 @@
     <t>Custos adicionais</t>
   </si>
   <si>
-    <t xml:space="preserve">Custo </t>
-  </si>
-  <si>
     <t>Valor</t>
   </si>
   <si>
@@ -83,33 +101,48 @@
   </si>
   <si>
     <t>Nargas</t>
+  </si>
+  <si>
+    <t>Custo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$R$ -416]#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -118,7 +151,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -176,27 +209,39 @@
     </fill>
   </fills>
   <borders count="23">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -206,6 +251,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -214,25 +260,33 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -244,16 +298,26 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-    </border>
-    <border>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -262,6 +326,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -276,38 +343,47 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FFB7E1CD"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FFB7E1CD"/>
       </top>
       <bottom style="thin">
         <color rgb="FFB7E1CD"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FFB7E1CD"/>
       </top>
       <bottom style="thin">
         <color rgb="FFB7E1CD"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FFB7E1CD"/>
       </right>
@@ -317,8 +393,10 @@
       <bottom style="thin">
         <color rgb="FFB7E1CD"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -328,22 +406,29 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -352,133 +437,125 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="39">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="4" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="7" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="4" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="7" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="6" fontId="3" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="16" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="18" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="19" fillId="7" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="20" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="11" fillId="9" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="10" fontId="3" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="7" fillId="10" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="10" fontId="3" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="10" fillId="10" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="10" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="18" fillId="10" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="10" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -668,292 +745,304 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="3">
         <v>81.25</v>
       </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="6">
         <v>80.75</v>
       </c>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="s">
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="6">
         <v>80.75</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="C5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="6">
         <v>80.75</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="8" t="s">
+      <c r="C6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="6">
         <v>80.75</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="8" t="s">
+      <c r="C7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="6">
         <v>81.25</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="8" t="s">
+      <c r="C8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="6">
         <v>81.25</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="8" t="s">
+      <c r="C9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="6">
         <v>81.25</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15" t="s">
+      <c r="C10" s="8"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17">
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="12">
         <f>SUM(B3+B4+B5+B6+B7+B8+B9+B10+B11+B12+B13+B14+B21+B22+B23)</f>
-        <v>892</v>
-      </c>
-      <c r="J10" s="18"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="8" t="s">
+        <v>1730</v>
+      </c>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="6">
         <v>40.75</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="8" t="s">
+      <c r="C11" s="8"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="6">
         <v>81.25</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="8" t="s">
+      <c r="C12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="6">
         <v>81.25</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="8" t="s">
+      <c r="C13" s="8"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="6">
         <v>40.75</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="11"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="11"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="20"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="21"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="24" t="s">
+      <c r="C14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="16"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="26"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="27" t="s">
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="C20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="28" t="s">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="29" t="s">
+      <c r="B21" s="22"/>
+      <c r="C21" s="23"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="32" t="s">
+      <c r="B22" s="25">
+        <v>50</v>
+      </c>
+      <c r="C22" s="26"/>
+    </row>
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
+      <c r="B23" s="28">
+        <v>788</v>
+      </c>
+      <c r="C23" s="29"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -966,6 +1055,7 @@
       <formula>LEN(TRIM(B3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>